<commit_message>
updating oil & gas validation logic
</commit_message>
<xml_diff>
--- a/feedback_forms/current_versions/oil_and_gas_operator_feedback_v070.xlsx
+++ b/feedback_forms/current_versions/oil_and_gas_operator_feedback_v070.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\one_drive\code\pycharm\feedback_portal\feedback_forms\current_versions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carb-my.sharepoint.com/personal/tony_held_arb_ca_gov/Documents/code/pycharm/feedback_portal/feedback_forms/current_versions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EE8268-DAE4-4909-A2E0-59640DD7E6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{88EE8268-DAE4-4909-A2E0-59640DD7E6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7AE94D9-A5C3-4FAD-B200-00C209FF3A11}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="17413" windowHeight="11467" xr2:uid="{AD2102A5-37B4-471F-BCEC-083B2F5B9811}"/>
+    <workbookView xWindow="-18120" yWindow="3410" windowWidth="17410" windowHeight="11470" xr2:uid="{AD2102A5-37B4-471F-BCEC-083B2F5B9811}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="5" r:id="rId1"/>
@@ -1666,7 +1666,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1840,6 +1840,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3029,8 +3032,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:AG76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.5"/>
@@ -4149,7 +4152,7 @@
       </c>
     </row>
     <row r="49" spans="2:33" s="10" customFormat="1" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B49" s="61" t="s">
+      <c r="B49" s="66" t="s">
         <v>26</v>
       </c>
       <c r="C49" s="44"/>
@@ -4617,7 +4620,7 @@
   <drawing r:id="rId4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3B9E63D1-6ADB-4B23-9D34-4B60AC2FE861}">
           <x14:formula1>
             <xm:f>_carb_only!$B$12:$B$14</xm:f>
@@ -6738,7 +6741,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A11" sqref="A11:R40"/>
     </sheetView>
   </sheetViews>
@@ -7348,30 +7351,11 @@
     <sortCondition ref="B1:B1048576"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E9A34E7C7C736409D4BDE6375CCC276" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cf521a6d855790dbe6a6d894ff439cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32" xmlns:ns3="e20ceb87-0d79-402a-b4b9-75d78589c76d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a45aa6d812898c4b0f52b4c3685679ce" ns2:_="" ns3:_="">
     <xsd:import namespace="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
@@ -7606,10 +7590,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{533C6BB5-3BBA-46E5-A63A-38A55F0F20F9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
+    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7626,20 +7641,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{533C6BB5-3BBA-46E5-A63A-38A55F0F20F9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
-    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>